<commit_message>
added verification point on flight search result page
</commit_message>
<xml_diff>
--- a/UnitedAirlineData.xlsx
+++ b/UnitedAirlineData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ola.ajala/Desktop/OwnProject/CompleteAutomationBootCamp/datadrivenframework/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-5120" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>from</t>
   </si>
@@ -89,6 +94,18 @@
   </si>
   <si>
     <t>Los Angeles, CA, US (LAX - All Airports)</t>
+  </si>
+  <si>
+    <t>Chicago, IL, US (CHI - All Airports)</t>
+  </si>
+  <si>
+    <t>New York, NY, US (NYC - All Airports)</t>
+  </si>
+  <si>
+    <t>Washington, DC, US (IAD - Dulles)</t>
+  </si>
+  <si>
+    <t>San Francisco, CA, US (SFO)</t>
   </si>
 </sst>
 </file>
@@ -505,14 +522,14 @@
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -558,7 +575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -581,7 +598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -606,11 +623,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -619,19 +631,19 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,12 +666,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -677,12 +689,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -700,7 +712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -725,10 +737,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>